<commit_message>
swap columns from details to header due to stupid decision.
</commit_message>
<xml_diff>
--- a/SqlQuery.xlsx
+++ b/SqlQuery.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YKW\AddOn-MasterTemplate-AYS_Production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YKW\AddOn-MasterTemplate-CHY_Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Code</t>
   </si>
@@ -44,9 +44,6 @@
     <t>salestype</t>
   </si>
   <si>
-    <t>select '1' as U_SalesType, '11' as name union all select '2' as U_SalesType, '22' as name</t>
-  </si>
-  <si>
     <t>Work_Order.grid2.U_SalesTyp.getData</t>
   </si>
   <si>
@@ -74,27 +71,18 @@
     <t>Work_Order.btnCopy.getSO</t>
   </si>
   <si>
-    <t>select top 3 ItemCode as U_ItemCode, FrgnName as U_ItemName, 'ABC' as U_Project from OITM where $[.U_SONo] = '1'</t>
-  </si>
-  <si>
     <t>Work_Order.grid1.U_ProdType.getData</t>
   </si>
   <si>
     <t>Production Type</t>
   </si>
   <si>
-    <t>select '1' as U_ProdType, '11' as name union all select '2' as U_SalesType, '22' as name</t>
-  </si>
-  <si>
     <t>Work_Order.grid1.U_Project.getData</t>
   </si>
   <si>
     <t>Project</t>
   </si>
   <si>
-    <t>select '1' as U_Project, '11' as name union all select '2' as U_SalesType, '22' as name</t>
-  </si>
-  <si>
     <t>Work_Order.grid2.U_ProdType.getData</t>
   </si>
   <si>
@@ -105,6 +93,51 @@
   </si>
   <si>
     <t>Project2</t>
+  </si>
+  <si>
+    <t>Work_Order.btnProj.getData</t>
+  </si>
+  <si>
+    <t>header Project</t>
+  </si>
+  <si>
+    <t>SELECT T0.[PrcCode] as U_Project, T0.[PrcName] FROM OPRC T0 WHERE T0.[DimCode] ='2' and  T0.[Active] ='Y'</t>
+  </si>
+  <si>
+    <t>Work_Order.btnSalesT.getData</t>
+  </si>
+  <si>
+    <t>salestype header</t>
+  </si>
+  <si>
+    <t>SELECT T0.[PrcCode] as U_SalesType, T0.[PrcName] FROM OPRC T0 WHERE T0.[DimCode] ='1' and  T0.[Active] ='Y'</t>
+  </si>
+  <si>
+    <t>Work_Order.grid1.U_Machine.getData</t>
+  </si>
+  <si>
+    <t>Machine1</t>
+  </si>
+  <si>
+    <t>select code as 'U_Machine', name from [@MACHINE]</t>
+  </si>
+  <si>
+    <t>select Code as U_ProdType,Name as name From [@FT_PRDTYPE]</t>
+  </si>
+  <si>
+    <t>Work_Order.grid2.U_Machine.getData</t>
+  </si>
+  <si>
+    <t>Machine2</t>
+  </si>
+  <si>
+    <t>Work_Order.grid3.U_Machine.getData</t>
+  </si>
+  <si>
+    <t>Machine3</t>
+  </si>
+  <si>
+    <t>select T1.DocNum as 'U_SONo',T1.DocDate,T1.NumAtCard as CustomerPONo,T2.ItemCode as U_ItemCode ,T2.U_DDesc as U_ItemName, T0.InvntryUom as 'U_UOM' , T2.Quantity as U_Quantity,T2.WhsCode as U_WhsCode,T2.U_Length as U_Length,T2.OcrCode2 as U_Project,T2.OcrCode as U_SalesType,T2.U_TotalW as U_Weight from ORDR T1 inner join RDR1 T2 on T1.DocEntry=T2.DocEntry inner join OITM T0 on T0.ItemCode = T2.ItemCode</t>
   </si>
 </sst>
 </file>
@@ -425,17 +458,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -449,106 +482,162 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>